<commit_message>
BOM and datasheets update
</commit_message>
<xml_diff>
--- a/BOM Light_system.xlsx
+++ b/BOM Light_system.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BasileBerckmoes\Documents\GitHub\Light_system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\school\KULeuven\jaar1\semester1\Elektronische tech Labo\Light_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50883EF-121D-4405-A54D-6CB18FD9F2F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{691B9DB8-9339-4958-89B7-511E31F3F689}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12015" yWindow="5310" windowWidth="22395" windowHeight="14460" xr2:uid="{C87271B4-23EB-4087-839C-EEF59018C3C7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{C87271B4-23EB-4087-839C-EEF59018C3C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Aantal</t>
   </si>
@@ -97,16 +97,35 @@
   </si>
   <si>
     <t xml:space="preserve">	2815636</t>
+  </si>
+  <si>
+    <t>LED, RGB, Red, Green, Blue, SMD, 2.4mm</t>
+  </si>
+  <si>
+    <t>ASMB-MTB1-0A3A2</t>
+  </si>
+  <si>
+    <t>Wire-To-Board Terminal Block, 2.5 mm, 12 Ways</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	PTSA0,5/12-2,5-Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -132,12 +151,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -153,8 +173,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BFA3D288-7921-423B-9F4D-B75D9CA6C0A3}" name="Table3" displayName="Table3" ref="A1:F17" totalsRowShown="0">
-  <autoFilter ref="A1:F17" xr:uid="{1DFD0A97-70DC-492C-9879-99DD55AE7A81}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{BFA3D288-7921-423B-9F4D-B75D9CA6C0A3}" name="Table3" displayName="Table3" ref="A1:F19" totalsRowShown="0">
+  <autoFilter ref="A1:F19" xr:uid="{1DFD0A97-70DC-492C-9879-99DD55AE7A81}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{DF49E3A0-0641-4903-8272-D343A8B811E1}" name="Aantal"/>
     <tableColumn id="2" xr3:uid="{9B813FAE-6E50-4889-B759-8F1CBBA9FB73}" name="Omschrijving"/>
@@ -168,7 +188,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -464,22 +484,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12DA10BB-9DB9-41F2-920B-05DCA4009D38}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="31.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -499,7 +519,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -516,7 +536,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -536,7 +556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -556,7 +576,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -576,7 +596,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -596,7 +616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -607,30 +627,71 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>
       </c>
       <c r="E9">
+        <v>0.38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>1.44</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11">
         <v>16.690000000000001</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F11" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Schema bucks & bom update
</commit_message>
<xml_diff>
--- a/BOM Light_system.xlsx
+++ b/BOM Light_system.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BasileBerckmoes\Documents\GitHub\Light_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{968788FA-01C0-41C0-9E5A-2BAB4BAA2B6E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16533083-BB92-4EB5-A2D0-7C6A0031BEB0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1140" windowWidth="15375" windowHeight="14460" xr2:uid="{C87271B4-23EB-4087-839C-EEF59018C3C7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C87271B4-23EB-4087-839C-EEF59018C3C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="47">
   <si>
     <t>Aantal</t>
   </si>
@@ -117,15 +117,6 @@
     <t>PTSA0,5/12-2,5-Z</t>
   </si>
   <si>
-    <t>Main 3,3Buck U1</t>
-  </si>
-  <si>
-    <t>Main 3,3Buck Cin</t>
-  </si>
-  <si>
-    <t>Main 3,3Buck Cout</t>
-  </si>
-  <si>
     <t>Panasonic 33μF 35V dc Hybrid Conductive Polymer Aluminium</t>
   </si>
   <si>
@@ -138,28 +129,49 @@
     <t xml:space="preserve">744-4980 </t>
   </si>
   <si>
-    <t>Main 3,3Buck L1</t>
-  </si>
-  <si>
     <t>131-1959</t>
   </si>
   <si>
     <t>SMD Resistor, 0805, 22 kohm, MC 1% Series, 150 V, Thick Film, 100 mW</t>
   </si>
   <si>
-    <t>Main 3,3Buck Rfbb</t>
-  </si>
-  <si>
     <t>SMD Chip Resistor, 0603, 100 kohm, 1% Series, 50 V, Thick Film, 63 mW</t>
   </si>
   <si>
-    <t>Main 3,3Buck Rfbt</t>
-  </si>
-  <si>
     <t>SMD Multilayer Ceramic Capacitor, 0.1 µF, 50 V, 0603</t>
   </si>
   <si>
-    <t>Main 3,3Buck Cbst</t>
+    <t>Main Buck Cbst</t>
+  </si>
+  <si>
+    <t>Main Buck Cout</t>
+  </si>
+  <si>
+    <t>Main Buck Cin</t>
+  </si>
+  <si>
+    <t>Main Buck U1</t>
+  </si>
+  <si>
+    <t>7447798271 -  Power Inductor (SMD), 27 µH</t>
+  </si>
+  <si>
+    <t>Main 5Buck L1</t>
+  </si>
+  <si>
+    <t>CPF0603F13K7C1 -  SMD Chip Resistor, 0603, 13.7 kohm</t>
+  </si>
+  <si>
+    <t>Main Buck Rfbt</t>
+  </si>
+  <si>
+    <t>Main 3.3Buck L2</t>
+  </si>
+  <si>
+    <t>Main 5buck Rfbb1</t>
+  </si>
+  <si>
+    <t>Main 3.3Buck Rfbb2</t>
   </si>
 </sst>
 </file>
@@ -541,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12DA10BB-9DB9-41F2-920B-05DCA4009D38}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -554,7 +566,7 @@
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -747,7 +759,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B12" t="s">
         <v>25</v>
@@ -762,12 +774,12 @@
         <v>1.56</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
@@ -782,27 +794,27 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="F13" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E14">
         <v>1.4119999999999999</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -810,19 +822,19 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="E15">
         <v>3.44</v>
       </c>
       <c r="F15" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -830,7 +842,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C16">
         <v>9332820</v>
@@ -842,7 +854,7 @@
         <v>0.52500000000000002</v>
       </c>
       <c r="F16" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -850,7 +862,7 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C17">
         <v>9330402</v>
@@ -862,7 +874,7 @@
         <v>0.751</v>
       </c>
       <c r="F17" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -870,7 +882,7 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C18">
         <v>2688469</v>
@@ -882,7 +894,47 @@
         <v>2.62</v>
       </c>
       <c r="F18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19">
+        <v>1800291</v>
+      </c>
+      <c r="D19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E19">
+        <v>3.77</v>
+      </c>
+      <c r="F19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
         <v>42</v>
+      </c>
+      <c r="C20">
+        <v>1527596</v>
+      </c>
+      <c r="D20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E20">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="F20" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
BOM changed, components added
</commit_message>
<xml_diff>
--- a/BOM Light_system.xlsx
+++ b/BOM Light_system.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\BasileBerckmoes\Documents\GitHub\Light_system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\school\KULeuven\jaar1\semester1\Elektronische tech Labo\Light_system\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{760C0AEE-9DC0-4AF2-932F-541ED91F8CE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BEFEDBA-95F4-4CF8-8C71-B0A88EF45F9A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C87271B4-23EB-4087-839C-EEF59018C3C7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{C87271B4-23EB-4087-839C-EEF59018C3C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
   <si>
     <t>Aantal</t>
   </si>
@@ -96,15 +96,6 @@
     <t>Main</t>
   </si>
   <si>
-    <t>LED, RGB, Red, Green, Blue, SMD, 2.4mm</t>
-  </si>
-  <si>
-    <t>ASMB-MTB1-0A3A2</t>
-  </si>
-  <si>
-    <t>Wire-To-Board Terminal Block, 2.5 mm, 12 Ways</t>
-  </si>
-  <si>
     <t>farnell</t>
   </si>
   <si>
@@ -114,9 +105,6 @@
     <t>SMD Multilayer Ceramic Capacitor, 10 µF, 50 V, 1210</t>
   </si>
   <si>
-    <t>PTSA0,5/12-2,5-Z</t>
-  </si>
-  <si>
     <t>Panasonic 33μF 35V dc Hybrid Conductive Polymer Aluminium</t>
   </si>
   <si>
@@ -181,6 +169,21 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>Standard LEDs - SMD 2220 PLCC4 Tricolor</t>
+  </si>
+  <si>
+    <t>ASMB-KTF0-0A306</t>
+  </si>
+  <si>
+    <t>Fixed Terminal Blocks PTSA 0.5/12-2.5-Z 12P 2.5MM 45DEG</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
 </sst>
 </file>
@@ -235,7 +238,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -267,7 +270,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -566,20 +569,20 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="65.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="2" max="2" width="65.33203125" customWidth="1"/>
+    <col min="3" max="3" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -599,10 +602,10 @@
         <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
@@ -618,8 +621,11 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -638,8 +644,11 @@
       <c r="F4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>1</v>
       </c>
@@ -658,8 +667,11 @@
       <c r="F5" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>2</v>
       </c>
@@ -678,8 +690,11 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -698,8 +713,11 @@
       <c r="F7" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -710,38 +728,41 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E9">
-        <v>0.38</v>
+        <v>0.22</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>27</v>
+        <v>49</v>
+      </c>
+      <c r="C10" s="2">
+        <v>1990106</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E10">
         <v>1.44</v>
@@ -749,8 +770,11 @@
       <c r="F10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -770,195 +794,195 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C12">
         <v>3007333</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E12">
         <v>1.56</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C13">
         <v>2094047</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E13">
         <v>2.2000000000000002</v>
       </c>
       <c r="F13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" t="s">
         <v>28</v>
       </c>
-      <c r="C14" t="s">
-        <v>32</v>
-      </c>
       <c r="D14" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E14">
         <v>1.4119999999999999</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E15">
         <v>3.44</v>
       </c>
       <c r="F15" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C16">
         <v>9332820</v>
       </c>
       <c r="D16" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E16">
         <v>0.52500000000000002</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C17">
         <v>9330402</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E17">
         <v>0.751</v>
       </c>
       <c r="F17" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C18">
         <v>2688469</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E18">
         <v>2.62</v>
       </c>
       <c r="F18" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C19">
         <v>1800291</v>
       </c>
       <c r="D19" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E19">
         <v>3.77</v>
       </c>
       <c r="F19" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C20">
         <v>1527596</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E20">
         <v>0.16800000000000001</v>
       </c>
       <c r="F20" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
PCB Main bijna af
</commit_message>
<xml_diff>
--- a/BOM Light_system.xlsx
+++ b/BOM Light_system.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Documents\school\KULeuven\jaar1\semester1\Elektronische tech Labo\Light_system\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/basileberckmoes/GitHub/Light_system/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4A7DB8-313F-4847-AE01-DEB911F01FFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B457D4B-3386-9F4E-B6D6-8E69A6CFC8CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{C87271B4-23EB-4087-839C-EEF59018C3C7}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12720" xr2:uid="{C87271B4-23EB-4087-839C-EEF59018C3C7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -566,20 +566,20 @@
   <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.33203125" customWidth="1"/>
     <col min="2" max="2" width="65.33203125" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" customWidth="1"/>
     <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -602,7 +602,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -622,7 +622,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>10</v>
       </c>
@@ -645,7 +645,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -668,7 +668,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -691,7 +691,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -714,7 +714,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -737,7 +737,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -760,7 +760,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -780,7 +780,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -800,7 +800,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -820,7 +820,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -840,7 +840,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -860,7 +860,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>10</v>
       </c>
@@ -880,7 +880,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>10</v>
       </c>
@@ -900,7 +900,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>10</v>
       </c>
@@ -920,7 +920,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -940,7 +940,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -960,7 +960,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>

</xml_diff>